<commit_message>
Close #17 and fix hardcoded round names
</commit_message>
<xml_diff>
--- a/seasons/RugbyUnion/MajorLeagueRugby/2023/forecasts/ReportRound6.xlsx
+++ b/seasons/RugbyUnion/MajorLeagueRugby/2023/forecasts/ReportRound6.xlsx
@@ -118,6 +118,15 @@
     <t>Houston, TX</t>
   </si>
   <si>
+    <t>UTAH</t>
+  </si>
+  <si>
+    <t>TOR</t>
+  </si>
+  <si>
+    <t>Herriman, UT</t>
+  </si>
+  <si>
     <t>CHI</t>
   </si>
   <si>
@@ -125,15 +134,6 @@
   </si>
   <si>
     <t>Bridgeview, IL</t>
-  </si>
-  <si>
-    <t>UTAH</t>
-  </si>
-  <si>
-    <t>TOR</t>
-  </si>
-  <si>
-    <t>Herriman, UT</t>
   </si>
 </sst>
 </file>
@@ -197,7 +197,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF63B445"/>
+      <color rgb="FFC81C22"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -205,7 +205,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFC81C22"/>
+      <color rgb="FF63B445"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -264,6 +264,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0D408B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF00653C"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -271,18 +283,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF182A55"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0D408B"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,16 +334,16 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -751,11 +751,11 @@
       </c>
       <c r="I3" s="13"/>
       <c r="K3" s="13">
-        <v>0.4892509403539777</v>
+        <v>0.1324999320622214</v>
       </c>
       <c r="L3" s="13"/>
       <c r="N3" s="13">
-        <v>0.1324999320622214</v>
+        <v>0.4892509403539777</v>
       </c>
       <c r="O3" s="13"/>
     </row>
@@ -764,23 +764,23 @@
         <v>2</v>
       </c>
       <c r="B4" s="13">
-        <v>0.03463299742015888</v>
+        <v>0.03486570345495707</v>
       </c>
       <c r="C4" s="13"/>
       <c r="E4" s="13">
-        <v>0.9658468156475116</v>
+        <v>0.9659600409376649</v>
       </c>
       <c r="F4" s="13"/>
       <c r="H4" s="13">
-        <v>0.3497329458893892</v>
+        <v>0.3494513174963016</v>
       </c>
       <c r="I4" s="13"/>
       <c r="K4" s="13">
-        <v>0.06400534767212367</v>
+        <v>0.7303307061449437</v>
       </c>
       <c r="L4" s="13"/>
       <c r="N4" s="13">
-        <v>0.7304710587196697</v>
+        <v>0.06397139186840474</v>
       </c>
       <c r="O4" s="13"/>
     </row>
@@ -789,23 +789,23 @@
         <v>3</v>
       </c>
       <c r="B5" s="12">
-        <v>1.755448146656069</v>
+        <v>1.767243353768706</v>
       </c>
       <c r="C5" s="12"/>
       <c r="E5" s="12">
-        <v>47.04725505515718</v>
+        <v>47.05277035946656</v>
       </c>
       <c r="F5" s="12"/>
       <c r="H5" s="12">
-        <v>23.86245921474523</v>
+        <v>23.84324356428177</v>
       </c>
       <c r="I5" s="12"/>
       <c r="K5" s="12">
-        <v>3.131467653626978</v>
+        <v>9.676876894715923</v>
       </c>
       <c r="L5" s="12"/>
       <c r="N5" s="12">
-        <v>9.678736565377518</v>
+        <v>3.129806362736982</v>
       </c>
       <c r="O5" s="12"/>
     </row>
@@ -814,34 +814,34 @@
         <v>4</v>
       </c>
       <c r="B6" s="14">
-        <v>0.9945302</v>
+        <v>0.9945311999999999</v>
       </c>
       <c r="C6" s="14">
-        <v>0.003621</v>
+        <v>0.0036498</v>
       </c>
       <c r="E6" s="14">
-        <v>0.570052</v>
+        <v>0.5700148</v>
       </c>
       <c r="F6" s="14">
-        <v>0.3669716</v>
+        <v>0.3672224</v>
       </c>
       <c r="H6" s="14">
-        <v>0.9143546</v>
+        <v>0.9145027999999999</v>
       </c>
       <c r="I6" s="14">
-        <v>0.0643152</v>
+        <v>0.0642486</v>
       </c>
       <c r="K6" s="14">
-        <v>0.0075212</v>
+        <v>0.776268</v>
       </c>
       <c r="L6" s="14">
-        <v>0.9899414</v>
+        <v>0.1992392</v>
       </c>
       <c r="N6" s="14">
-        <v>0.7763914</v>
+        <v>0.0075164</v>
       </c>
       <c r="O6" s="14">
-        <v>0.1993586</v>
+        <v>0.9899476</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -849,34 +849,34 @@
         <v>5</v>
       </c>
       <c r="B7" s="15">
-        <v>35.11968</v>
+        <v>35.1190718</v>
       </c>
       <c r="C7" s="15">
-        <v>13.82933</v>
+        <v>13.82852</v>
       </c>
       <c r="E7" s="15">
-        <v>28.0202138</v>
+        <v>28.0165104</v>
       </c>
       <c r="F7" s="15">
-        <v>25.3747006</v>
+        <v>25.3710078</v>
       </c>
       <c r="H7" s="15">
-        <v>28.149035</v>
+        <v>28.1554178</v>
       </c>
       <c r="I7" s="15">
-        <v>17.1406292</v>
+        <v>17.1412582</v>
       </c>
       <c r="K7" s="15">
-        <v>11.6837428</v>
+        <v>24.444969</v>
       </c>
       <c r="L7" s="15">
-        <v>34.4120662</v>
+        <v>16.2451552</v>
       </c>
       <c r="N7" s="15">
-        <v>24.4428008</v>
+        <v>11.6851326</v>
       </c>
       <c r="O7" s="15">
-        <v>16.2478214</v>
+        <v>34.4049178</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -902,16 +902,16 @@
         <v>10</v>
       </c>
       <c r="K8" s="15">
+        <v>12</v>
+      </c>
+      <c r="L8" s="15">
+        <v>5</v>
+      </c>
+      <c r="N8" s="15">
         <v>6</v>
       </c>
-      <c r="L8" s="15">
-        <v>23</v>
-      </c>
-      <c r="N8" s="15">
-        <v>12</v>
-      </c>
       <c r="O8" s="15">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -937,16 +937,16 @@
         <v>12</v>
       </c>
       <c r="K9" s="15">
+        <v>14</v>
+      </c>
+      <c r="L9" s="15">
+        <v>7</v>
+      </c>
+      <c r="N9" s="15">
         <v>6</v>
       </c>
-      <c r="L9" s="15">
+      <c r="O9" s="15">
         <v>25</v>
-      </c>
-      <c r="N9" s="15">
-        <v>14</v>
-      </c>
-      <c r="O9" s="15">
-        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -972,16 +972,16 @@
         <v>12</v>
       </c>
       <c r="K10" s="15">
+        <v>17</v>
+      </c>
+      <c r="L10" s="15">
+        <v>8</v>
+      </c>
+      <c r="N10" s="15">
         <v>6</v>
       </c>
-      <c r="L10" s="15">
+      <c r="O10" s="15">
         <v>27</v>
-      </c>
-      <c r="N10" s="15">
-        <v>17</v>
-      </c>
-      <c r="O10" s="15">
-        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1007,16 +1007,16 @@
         <v>13</v>
       </c>
       <c r="K11" s="15">
+        <v>19</v>
+      </c>
+      <c r="L11" s="15">
+        <v>10</v>
+      </c>
+      <c r="N11" s="15">
         <v>6</v>
       </c>
-      <c r="L11" s="15">
+      <c r="O11" s="15">
         <v>28</v>
-      </c>
-      <c r="N11" s="15">
-        <v>19</v>
-      </c>
-      <c r="O11" s="15">
-        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1042,16 +1042,16 @@
         <v>14</v>
       </c>
       <c r="K12" s="15">
+        <v>19</v>
+      </c>
+      <c r="L12" s="15">
+        <v>11</v>
+      </c>
+      <c r="N12" s="15">
         <v>9</v>
       </c>
-      <c r="L12" s="15">
+      <c r="O12" s="15">
         <v>30</v>
-      </c>
-      <c r="N12" s="15">
-        <v>19</v>
-      </c>
-      <c r="O12" s="15">
-        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1077,16 +1077,16 @@
         <v>15</v>
       </c>
       <c r="K13" s="15">
+        <v>21</v>
+      </c>
+      <c r="L13" s="15">
+        <v>12</v>
+      </c>
+      <c r="N13" s="15">
         <v>9</v>
       </c>
-      <c r="L13" s="15">
+      <c r="O13" s="15">
         <v>31</v>
-      </c>
-      <c r="N13" s="15">
-        <v>21</v>
-      </c>
-      <c r="O13" s="15">
-        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -1112,16 +1112,16 @@
         <v>16</v>
       </c>
       <c r="K14" s="15">
+        <v>22</v>
+      </c>
+      <c r="L14" s="15">
+        <v>13</v>
+      </c>
+      <c r="N14" s="15">
         <v>9</v>
       </c>
-      <c r="L14" s="15">
+      <c r="O14" s="15">
         <v>32</v>
-      </c>
-      <c r="N14" s="15">
-        <v>22</v>
-      </c>
-      <c r="O14" s="15">
-        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1147,16 +1147,16 @@
         <v>17</v>
       </c>
       <c r="K15" s="15">
+        <v>22</v>
+      </c>
+      <c r="L15" s="15">
+        <v>14</v>
+      </c>
+      <c r="N15" s="15">
         <v>9</v>
       </c>
-      <c r="L15" s="15">
+      <c r="O15" s="15">
         <v>33</v>
-      </c>
-      <c r="N15" s="15">
-        <v>22</v>
-      </c>
-      <c r="O15" s="15">
-        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1182,16 +1182,16 @@
         <v>17</v>
       </c>
       <c r="K16" s="15">
+        <v>24</v>
+      </c>
+      <c r="L16" s="15">
+        <v>15</v>
+      </c>
+      <c r="N16" s="15">
         <v>9</v>
       </c>
-      <c r="L16" s="15">
+      <c r="O16" s="15">
         <v>34</v>
-      </c>
-      <c r="N16" s="15">
-        <v>24</v>
-      </c>
-      <c r="O16" s="15">
-        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1217,16 +1217,16 @@
         <v>17</v>
       </c>
       <c r="K17" s="15">
+        <v>25</v>
+      </c>
+      <c r="L17" s="15">
+        <v>16</v>
+      </c>
+      <c r="N17" s="15">
         <v>10</v>
       </c>
-      <c r="L17" s="15">
+      <c r="O17" s="15">
         <v>35</v>
-      </c>
-      <c r="N17" s="15">
-        <v>25</v>
-      </c>
-      <c r="O17" s="15">
-        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1252,16 +1252,16 @@
         <v>19</v>
       </c>
       <c r="K18" s="15">
+        <v>26</v>
+      </c>
+      <c r="L18" s="15">
+        <v>17</v>
+      </c>
+      <c r="N18" s="15">
         <v>12</v>
       </c>
-      <c r="L18" s="15">
+      <c r="O18" s="15">
         <v>36</v>
-      </c>
-      <c r="N18" s="15">
-        <v>26</v>
-      </c>
-      <c r="O18" s="15">
-        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -1287,16 +1287,16 @@
         <v>19</v>
       </c>
       <c r="K19" s="15">
+        <v>26</v>
+      </c>
+      <c r="L19" s="15">
+        <v>18</v>
+      </c>
+      <c r="N19" s="15">
         <v>13</v>
       </c>
-      <c r="L19" s="15">
+      <c r="O19" s="15">
         <v>36</v>
-      </c>
-      <c r="N19" s="15">
-        <v>26</v>
-      </c>
-      <c r="O19" s="15">
-        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -1322,16 +1322,16 @@
         <v>19</v>
       </c>
       <c r="K20" s="15">
+        <v>28</v>
+      </c>
+      <c r="L20" s="15">
+        <v>19</v>
+      </c>
+      <c r="N20" s="15">
         <v>13</v>
       </c>
-      <c r="L20" s="15">
+      <c r="O20" s="15">
         <v>37</v>
-      </c>
-      <c r="N20" s="15">
-        <v>28</v>
-      </c>
-      <c r="O20" s="15">
-        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -1357,16 +1357,16 @@
         <v>19</v>
       </c>
       <c r="K21" s="15">
+        <v>28</v>
+      </c>
+      <c r="L21" s="15">
+        <v>20</v>
+      </c>
+      <c r="N21" s="15">
         <v>14</v>
       </c>
-      <c r="L21" s="15">
+      <c r="O21" s="15">
         <v>38</v>
-      </c>
-      <c r="N21" s="15">
-        <v>28</v>
-      </c>
-      <c r="O21" s="15">
-        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1392,16 +1392,16 @@
         <v>20</v>
       </c>
       <c r="K22" s="15">
+        <v>29</v>
+      </c>
+      <c r="L22" s="15">
+        <v>21</v>
+      </c>
+      <c r="N22" s="15">
         <v>16</v>
       </c>
-      <c r="L22" s="15">
+      <c r="O22" s="15">
         <v>39</v>
-      </c>
-      <c r="N22" s="15">
-        <v>29</v>
-      </c>
-      <c r="O22" s="15">
-        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -1427,16 +1427,16 @@
         <v>21</v>
       </c>
       <c r="K23" s="15">
+        <v>31</v>
+      </c>
+      <c r="L23" s="15">
+        <v>23</v>
+      </c>
+      <c r="N23" s="15">
         <v>16</v>
       </c>
-      <c r="L23" s="15">
+      <c r="O23" s="15">
         <v>40</v>
-      </c>
-      <c r="N23" s="15">
-        <v>31</v>
-      </c>
-      <c r="O23" s="15">
-        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -1462,16 +1462,16 @@
         <v>21</v>
       </c>
       <c r="K24" s="15">
+        <v>32</v>
+      </c>
+      <c r="L24" s="15">
+        <v>24</v>
+      </c>
+      <c r="N24" s="15">
         <v>16</v>
       </c>
-      <c r="L24" s="15">
+      <c r="O24" s="15">
         <v>42</v>
-      </c>
-      <c r="N24" s="15">
-        <v>32</v>
-      </c>
-      <c r="O24" s="15">
-        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -1497,16 +1497,16 @@
         <v>22</v>
       </c>
       <c r="K25" s="15">
+        <v>33</v>
+      </c>
+      <c r="L25" s="15">
+        <v>26</v>
+      </c>
+      <c r="N25" s="15">
         <v>19</v>
       </c>
-      <c r="L25" s="15">
+      <c r="O25" s="15">
         <v>43</v>
-      </c>
-      <c r="N25" s="15">
-        <v>33</v>
-      </c>
-      <c r="O25" s="15">
-        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:15">
@@ -1532,16 +1532,16 @@
         <v>24</v>
       </c>
       <c r="K26" s="15">
+        <v>35</v>
+      </c>
+      <c r="L26" s="15">
+        <v>29</v>
+      </c>
+      <c r="N26" s="15">
         <v>21</v>
       </c>
-      <c r="L26" s="15">
+      <c r="O26" s="15">
         <v>46</v>
-      </c>
-      <c r="N26" s="15">
-        <v>35</v>
-      </c>
-      <c r="O26" s="15">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>